<commit_message>
Added a second excel spreadsheet used for our project and did more data manipulation within the excel file to make the scatter plot clearer
</commit_message>
<xml_diff>
--- a/Final Project Best Dataset/Newest EDV Project Dataset BWS.xlsx
+++ b/Final Project Best Dataset/Newest EDV Project Dataset BWS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14127\Downloads\Env Data Vis\HW9\Final Project Best Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C9D2214-C0BF-43AB-9598-469F431DB1E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE71E051-09AF-47B3-AD69-BD1A6B19B2DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Newest EDV Project Dataset" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="125">
   <si>
     <t>County_Name</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>LogWells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log violations </t>
   </si>
 </sst>
 </file>
@@ -3583,16 +3586,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>211137</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>277812</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3960,7 +3963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -15938,15 +15941,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D62DDBE-7B2C-4CF4-9CF7-39C5DE8A91ED}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15956,8 +15959,14 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -15967,8 +15976,15 @@
       <c r="D2">
         <v>37.338000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F2">
+        <f>LOG(C2 +0.1)</f>
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>37.338000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -15978,8 +15994,15 @@
       <c r="D3">
         <v>30.433</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">LOG(C3 +0.1)</f>
+        <v>0.61278385671973545</v>
+      </c>
+      <c r="G3">
+        <v>30.433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -15989,8 +16012,15 @@
       <c r="D4">
         <v>42.658999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.8202014594856402</v>
+      </c>
+      <c r="G4">
+        <v>42.658999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -16000,8 +16030,15 @@
       <c r="D5">
         <v>39.018000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.3222192947339193</v>
+      </c>
+      <c r="G5">
+        <v>39.018000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -16011,8 +16048,15 @@
       <c r="D6">
         <v>42.978000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>42.978000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -16022,8 +16066,15 @@
       <c r="D7">
         <v>33.555</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>33.555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -16033,8 +16084,15 @@
       <c r="D8">
         <v>39.972999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.1789769472931695</v>
+      </c>
+      <c r="G8">
+        <v>39.972999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -16044,8 +16102,15 @@
       <c r="D9">
         <v>38.417000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.8837182019639598</v>
+      </c>
+      <c r="G9">
+        <v>38.417000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -16055,8 +16120,15 @@
       <c r="D10">
         <v>32.225000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>32.225000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -16066,8 +16138,15 @@
       <c r="D11">
         <v>38.97</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1.7566361082458481</v>
+      </c>
+      <c r="G11">
+        <v>38.97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -16077,8 +16156,15 @@
       <c r="D12">
         <v>39.054000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>39.054000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -16088,8 +16174,15 @@
       <c r="D13">
         <v>39.932000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1.7489628612561614</v>
+      </c>
+      <c r="G13">
+        <v>39.932000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -16099,8 +16192,15 @@
       <c r="D14">
         <v>37.790999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <v>37.790999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -16110,8 +16210,15 @@
       <c r="D15">
         <v>31.113</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1.4927603890268375</v>
+      </c>
+      <c r="G15">
+        <v>31.113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -16121,8 +16228,15 @@
       <c r="D16">
         <v>31.753</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <v>31.753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -16132,8 +16246,15 @@
       <c r="D17">
         <v>40.085999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1.7084209001347128</v>
+      </c>
+      <c r="G17">
+        <v>40.085999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -16143,8 +16264,15 @@
       <c r="D18">
         <v>40.081000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1.8267225201689921</v>
+      </c>
+      <c r="G18">
+        <v>40.081000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -16154,8 +16282,15 @@
       <c r="D19">
         <v>36.601999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.8068580295188175</v>
+      </c>
+      <c r="G19">
+        <v>36.601999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -16165,8 +16300,15 @@
       <c r="D20">
         <v>39.421999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>39.421999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -16176,8 +16318,15 @@
       <c r="D21">
         <v>36.954000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.85125834871907524</v>
+      </c>
+      <c r="G21">
+        <v>36.954000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -16187,8 +16336,15 @@
       <c r="D22">
         <v>34.704000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G22">
+        <v>34.704000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -16198,8 +16354,15 @@
       <c r="D23">
         <v>31.742999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G23">
+        <v>31.742999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -16209,8 +16372,15 @@
       <c r="D24">
         <v>29.85</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G24">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -16220,8 +16390,15 @@
       <c r="D25">
         <v>40.078000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1.3996737214810382</v>
+      </c>
+      <c r="G25">
+        <v>40.078000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -16231,8 +16408,15 @@
       <c r="D26">
         <v>34.119999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G26">
+        <v>34.119999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -16242,8 +16426,15 @@
       <c r="D27">
         <v>40.212000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1.5921767573958667</v>
+      </c>
+      <c r="G27">
+        <v>40.212000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -16253,8 +16444,15 @@
       <c r="D28">
         <v>39.582000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>1.2068258760318498</v>
+      </c>
+      <c r="G28">
+        <v>39.582000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -16264,8 +16462,15 @@
       <c r="D29">
         <v>39.805</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G29">
+        <v>39.805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -16275,8 +16480,15 @@
       <c r="D30">
         <v>43.064999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G30">
+        <v>43.064999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -16286,8 +16498,15 @@
       <c r="D31">
         <v>47.218000000000004</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>2.0457140589408676</v>
+      </c>
+      <c r="G31">
+        <v>47.218000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -16297,8 +16516,15 @@
       <c r="D32">
         <v>40.201000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.3222192947339193</v>
+      </c>
+      <c r="G32">
+        <v>40.201000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -16308,8 +16534,15 @@
       <c r="D33">
         <v>45.811999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.1172712956557642</v>
+      </c>
+      <c r="G33">
+        <v>45.811999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -16319,8 +16552,15 @@
       <c r="D34">
         <v>41.372</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1.7331972651065695</v>
+      </c>
+      <c r="G34">
+        <v>41.372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -16330,8 +16570,15 @@
       <c r="D35">
         <v>40.880000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G35">
+        <v>40.880000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -16341,8 +16588,15 @@
       <c r="D36">
         <v>34.095999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G36">
+        <v>34.095999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -16352,8 +16606,15 @@
       <c r="D37">
         <v>34.835999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G37">
+        <v>34.835999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -16363,8 +16624,15 @@
       <c r="D38">
         <v>38.988999999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1.1172712956557642</v>
+      </c>
+      <c r="G38">
+        <v>38.988999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -16374,8 +16642,15 @@
       <c r="D39">
         <v>38.140999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G39">
+        <v>38.140999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -16385,8 +16660,15 @@
       <c r="D40">
         <v>31.143999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G40">
+        <v>31.143999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -16396,8 +16678,15 @@
       <c r="D41">
         <v>36.359000000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G41">
+        <v>36.359000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -16407,8 +16696,15 @@
       <c r="D42">
         <v>37.93</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>2.8035253955765325</v>
+      </c>
+      <c r="G42">
+        <v>37.93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -16418,8 +16714,15 @@
       <c r="D43">
         <v>39.872</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1.5453071164658241</v>
+      </c>
+      <c r="G43">
+        <v>39.872</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -16429,8 +16732,15 @@
       <c r="D44">
         <v>38.365000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>1.2329961103921538</v>
+      </c>
+      <c r="G44">
+        <v>38.365000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -16440,8 +16750,15 @@
       <c r="D45">
         <v>40.624000000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G45">
+        <v>40.624000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -16451,8 +16768,15 @@
       <c r="D46">
         <v>32.832000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G46">
+        <v>32.832000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -16462,8 +16786,15 @@
       <c r="D47">
         <v>30.175999999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G47">
+        <v>30.175999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -16473,8 +16804,15 @@
       <c r="D48">
         <v>43.390999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G48">
+        <v>43.390999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -16484,8 +16822,15 @@
       <c r="D49">
         <v>32.932000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G49">
+        <v>32.932000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -16495,8 +16840,15 @@
       <c r="D50">
         <v>39.366</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G50">
+        <v>39.366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -16506,8 +16858,15 @@
       <c r="D51">
         <v>39.994999999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G51">
+        <v>39.994999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -16517,8 +16876,15 @@
       <c r="D52">
         <v>24.704000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G52">
+        <v>24.704000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -16528,8 +16894,15 @@
       <c r="D53">
         <v>35.277999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G53">
+        <v>35.277999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -16539,8 +16912,15 @@
       <c r="D54">
         <v>41.43</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>2.0378247505883418</v>
+      </c>
+      <c r="G54">
+        <v>41.43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -16550,8 +16930,15 @@
       <c r="D55">
         <v>40.159999999999997</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G55">
+        <v>40.159999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -16561,8 +16948,15 @@
       <c r="D56">
         <v>37.911999999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G56">
+        <v>37.911999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -16572,8 +16966,15 @@
       <c r="D57">
         <v>41.578000000000003</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0.95904139232109353</v>
+      </c>
+      <c r="G57">
+        <v>41.578000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -16583,8 +16984,15 @@
       <c r="D58">
         <v>39.829000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>1.909020854211156</v>
+      </c>
+      <c r="G58">
+        <v>39.829000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -16594,8 +17002,15 @@
       <c r="D59">
         <v>39.206000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>2.9004217534577377</v>
+      </c>
+      <c r="G59">
+        <v>39.206000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -16605,8 +17020,15 @@
       <c r="D60">
         <v>40.344999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>2.7050936105478733</v>
+      </c>
+      <c r="G60">
+        <v>40.344999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -16616,8 +17038,15 @@
       <c r="D61">
         <v>35.170999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G61">
+        <v>35.170999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -16627,8 +17056,15 @@
       <c r="D62">
         <v>39.383000000000003</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0.85125834871907524</v>
+      </c>
+      <c r="G62">
+        <v>39.383000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -16638,8 +17074,15 @@
       <c r="D63">
         <v>40.200000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G63">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -16649,8 +17092,15 @@
       <c r="D64">
         <v>38.412999999999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>2.1849751906982608</v>
+      </c>
+      <c r="G64">
+        <v>38.412999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -16660,8 +17110,15 @@
       <c r="D65">
         <v>37.645000000000003</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G65">
+        <v>37.645000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>117</v>
       </c>
@@ -16671,8 +17128,15 @@
       <c r="D66">
         <v>39.076000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>1.7566361082458481</v>
+      </c>
+      <c r="G66">
+        <v>39.076000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -16682,8 +17146,15 @@
       <c r="D67">
         <v>39.006</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F67">
+        <f t="shared" ref="F67:F68" si="1">LOG(C67 +0.1)</f>
+        <v>2.1525940779274699</v>
+      </c>
+      <c r="G67">
+        <v>39.006</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -16691,6 +17162,13 @@
         <v>0</v>
       </c>
       <c r="D68">
+        <v>36.075000000000003</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G68">
         <v>36.075000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more changes! playing with the bubble plot
</commit_message>
<xml_diff>
--- a/Final Project Best Dataset/Newest EDV Project Dataset BWS.xlsx
+++ b/Final Project Best Dataset/Newest EDV Project Dataset BWS.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14127\Downloads\Env Data Vis\HW9\Final Project Best Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg2362\Dropbox (Yale_FES)\2_year\Spring_2021\Data_Viz\Assignment9\HW9\Final Project Best Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE71E051-09AF-47B3-AD69-BD1A6B19B2DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19380" windowHeight="10380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Newest EDV Project Dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Trust Vs Violations" sheetId="3" r:id="rId2"/>
     <sheet name="Richer Counties" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -413,7 +412,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -936,7 +935,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -950,6 +949,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1506,7 +1506,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A25E-4320-B615-8983CAE4A02B}"/>
             </c:ext>
@@ -1520,11 +1520,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1623575520"/>
-        <c:axId val="1623572608"/>
+        <c:axId val="-565981632"/>
+        <c:axId val="-565995776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1623575520"/>
+        <c:axId val="-565981632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,12 +1581,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1623572608"/>
+        <c:crossAx val="-565995776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1623572608"/>
+        <c:axId val="-565995776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1623575520"/>
+        <c:crossAx val="-565981632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1693,7 +1693,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1742,6 +1742,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2284,7 +2285,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-099F-406D-AAAB-EA5637737207}"/>
             </c:ext>
@@ -2298,11 +2299,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="345890880"/>
-        <c:axId val="345892128"/>
+        <c:axId val="-565989792"/>
+        <c:axId val="-565989248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="345890880"/>
+        <c:axId val="-565989792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2359,12 +2360,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345892128"/>
+        <c:crossAx val="-565989248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="345892128"/>
+        <c:axId val="-565989248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2421,7 +2422,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345890880"/>
+        <c:crossAx val="-565989792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3586,13 +3587,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>277812</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -3602,7 +3603,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F138B32C-8807-4CB2-8AE4-26394CF2B21F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F138B32C-8807-4CB2-8AE4-26394CF2B21F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3643,7 +3644,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B476A24-347F-4E5F-BD42-8E4FEB7A7D26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B476A24-347F-4E5F-BD42-8E4FEB7A7D26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3960,16 +3961,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -4318,7 +4319,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -4494,7 +4495,7 @@
         <v>1.8000293592441343</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -4670,7 +4671,7 @@
         <v>2.3055663135153042</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>1.4785664955938433</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -5022,7 +5023,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -5198,7 +5199,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -5374,7 +5375,7 @@
         <v>0.78532983501076703</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -5550,7 +5551,7 @@
         <v>3.040246215057707</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -5726,7 +5727,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -5902,7 +5903,7 @@
         <v>2.5066403055665027</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>0.49136169383427269</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -6254,7 +6255,7 @@
         <v>1.6344772701607315</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -6430,7 +6431,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -6606,7 +6607,7 @@
         <v>1.4166405073382811</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -6958,7 +6959,7 @@
         <v>1.3820170425748683</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -7134,7 +7135,7 @@
         <v>2.0090257420869104</v>
       </c>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -7310,7 +7311,7 @@
         <v>1.8457180179666586</v>
       </c>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -7486,7 +7487,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -7662,7 +7663,7 @@
         <v>0.49136169383427269</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -7838,7 +7839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -8014,7 +8015,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -8190,7 +8191,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -8366,7 +8367,7 @@
         <v>1.7788744720027396</v>
       </c>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -8542,7 +8543,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -8718,7 +8719,7 @@
         <v>2.4101020766428607</v>
       </c>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -8894,7 +8895,7 @@
         <v>1.1492191126553799</v>
       </c>
     </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -9070,7 +9071,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -9246,7 +9247,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -9422,7 +9423,7 @@
         <v>2.9395691686559018</v>
       </c>
     </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -9598,7 +9599,7 @@
         <v>4.1392685158225077E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -9774,7 +9775,7 @@
         <v>1.5198279937757189</v>
       </c>
     </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -9950,7 +9951,7 @@
         <v>1.6910814921229684</v>
       </c>
     </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -10126,7 +10127,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -10302,7 +10303,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -10478,7 +10479,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -10654,7 +10655,7 @@
         <v>1.7168377232995244</v>
       </c>
     </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -10830,7 +10831,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -11006,7 +11007,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -11182,7 +11183,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -11358,7 +11359,7 @@
         <v>2.9201755220100227</v>
       </c>
     </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -11534,7 +11535,7 @@
         <v>1.8135809885681919</v>
       </c>
     </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -11710,7 +11711,7 @@
         <v>1.5809249756756194</v>
       </c>
     </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -11886,7 +11887,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -12062,7 +12063,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -12238,7 +12239,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -12414,7 +12415,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -12590,7 +12591,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -12766,7 +12767,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -12942,7 +12943,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -13118,7 +13119,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -13294,7 +13295,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -13470,7 +13471,7 @@
         <v>1.6031443726201824</v>
       </c>
     </row>
-    <row r="55" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -13646,7 +13647,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -13822,7 +13823,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -13998,7 +13999,7 @@
         <v>1.2329961103921538</v>
       </c>
     </row>
-    <row r="58" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -14174,7 +14175,7 @@
         <v>1.9916690073799486</v>
       </c>
     </row>
-    <row r="59" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -14350,7 +14351,7 @@
         <v>3.0330616925381735</v>
       </c>
     </row>
-    <row r="60" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -14526,7 +14527,7 @@
         <v>2.8202671571609645</v>
       </c>
     </row>
-    <row r="61" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -14702,7 +14703,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -14878,7 +14879,7 @@
         <v>0.61278385671973545</v>
       </c>
     </row>
-    <row r="63" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -15054,7 +15055,7 @@
         <v>0.49136169383427269</v>
       </c>
     </row>
-    <row r="64" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -15230,7 +15231,7 @@
         <v>3.0592225125296895</v>
       </c>
     </row>
-    <row r="65" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -15406,7 +15407,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>117</v>
       </c>
@@ -15582,7 +15583,7 @@
         <v>2.3998467127129226</v>
       </c>
     </row>
-    <row r="67" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -15758,7 +15759,7 @@
         <v>2.3581252852766488</v>
       </c>
     </row>
-    <row r="68" spans="1:59" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -15940,16 +15941,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D62DDBE-7B2C-4CF4-9CF7-39C5DE8A91ED}">
-  <dimension ref="A1:G68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.09765625" customWidth="1"/>
+    <col min="4" max="4" width="18.796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15959,14 +15964,14 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
       <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -15976,15 +15981,15 @@
       <c r="D2">
         <v>37.338000000000001</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <f>LOG(C2 +0.1)</f>
         <v>-1</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>37.338000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -15994,15 +15999,15 @@
       <c r="D3">
         <v>30.433</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">LOG(C3 +0.1)</f>
+        <v>0.61278385671973545</v>
+      </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">LOG(C3 +0.1)</f>
-        <v>0.61278385671973545</v>
-      </c>
-      <c r="G3">
         <v>30.433</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -16012,15 +16017,15 @@
       <c r="D4">
         <v>42.658999999999999</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>1.8202014594856402</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>42.658999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -16030,15 +16035,15 @@
       <c r="D5">
         <v>39.018000000000001</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>0.3222192947339193</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>39.018000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -16048,15 +16053,15 @@
       <c r="D6">
         <v>42.978000000000002</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>42.978000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -16066,15 +16071,15 @@
       <c r="D7">
         <v>33.555</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <v>33.555</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -16084,15 +16089,15 @@
       <c r="D8">
         <v>39.972999999999999</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1.1789769472931695</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>39.972999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -16102,15 +16107,15 @@
       <c r="D9">
         <v>38.417000000000002</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>2.8837182019639598</v>
       </c>
-      <c r="G9">
+      <c r="F9">
         <v>38.417000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -16120,15 +16125,15 @@
       <c r="D10">
         <v>32.225000000000001</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <v>32.225000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -16138,15 +16143,15 @@
       <c r="D11">
         <v>38.97</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>1.7566361082458481</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <v>38.97</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -16156,15 +16161,15 @@
       <c r="D12">
         <v>39.054000000000002</v>
       </c>
-      <c r="F12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>39.054000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -16174,15 +16179,15 @@
       <c r="D13">
         <v>39.932000000000002</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>1.7489628612561614</v>
       </c>
-      <c r="G13">
+      <c r="F13">
         <v>39.932000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -16192,15 +16197,15 @@
       <c r="D14">
         <v>37.790999999999997</v>
       </c>
-      <c r="F14">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G14">
+      <c r="F14">
         <v>37.790999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -16210,15 +16215,15 @@
       <c r="D15">
         <v>31.113</v>
       </c>
-      <c r="F15">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>1.4927603890268375</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <v>31.113</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -16228,15 +16233,15 @@
       <c r="D16">
         <v>31.753</v>
       </c>
-      <c r="F16">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G16">
+      <c r="F16">
         <v>31.753</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -16246,15 +16251,15 @@
       <c r="D17">
         <v>40.085999999999999</v>
       </c>
-      <c r="F17">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>1.7084209001347128</v>
       </c>
-      <c r="G17">
+      <c r="F17">
         <v>40.085999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -16264,15 +16269,15 @@
       <c r="D18">
         <v>40.081000000000003</v>
       </c>
-      <c r="F18">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>1.8267225201689921</v>
       </c>
-      <c r="G18">
+      <c r="F18">
         <v>40.081000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -16282,15 +16287,15 @@
       <c r="D19">
         <v>36.601999999999997</v>
       </c>
-      <c r="F19">
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>1.8068580295188175</v>
       </c>
-      <c r="G19">
+      <c r="F19">
         <v>36.601999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -16300,15 +16305,15 @@
       <c r="D20">
         <v>39.421999999999997</v>
       </c>
-      <c r="F20">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G20">
+      <c r="F20">
         <v>39.421999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -16318,15 +16323,15 @@
       <c r="D21">
         <v>36.954000000000001</v>
       </c>
-      <c r="F21">
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>0.85125834871907524</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>36.954000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -16336,15 +16341,15 @@
       <c r="D22">
         <v>34.704000000000001</v>
       </c>
-      <c r="F22">
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G22">
+      <c r="F22">
         <v>34.704000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -16354,15 +16359,15 @@
       <c r="D23">
         <v>31.742999999999999</v>
       </c>
-      <c r="F23">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G23">
+      <c r="F23">
         <v>31.742999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -16372,15 +16377,15 @@
       <c r="D24">
         <v>29.85</v>
       </c>
-      <c r="F24">
+      <c r="E24">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G24">
+      <c r="F24">
         <v>29.85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -16390,15 +16395,15 @@
       <c r="D25">
         <v>40.078000000000003</v>
       </c>
-      <c r="F25">
+      <c r="E25">
         <f t="shared" si="0"/>
         <v>1.3996737214810382</v>
       </c>
-      <c r="G25">
+      <c r="F25">
         <v>40.078000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -16408,15 +16413,15 @@
       <c r="D26">
         <v>34.119999999999997</v>
       </c>
-      <c r="F26">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G26">
+      <c r="F26">
         <v>34.119999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -16426,15 +16431,15 @@
       <c r="D27">
         <v>40.212000000000003</v>
       </c>
-      <c r="F27">
+      <c r="E27">
         <f t="shared" si="0"/>
         <v>1.5921767573958667</v>
       </c>
-      <c r="G27">
+      <c r="F27">
         <v>40.212000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -16444,15 +16449,15 @@
       <c r="D28">
         <v>39.582000000000001</v>
       </c>
-      <c r="F28">
+      <c r="E28">
         <f t="shared" si="0"/>
         <v>1.2068258760318498</v>
       </c>
-      <c r="G28">
+      <c r="F28">
         <v>39.582000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -16462,15 +16467,15 @@
       <c r="D29">
         <v>39.805</v>
       </c>
-      <c r="F29">
+      <c r="E29">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G29">
+      <c r="F29">
         <v>39.805</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -16480,15 +16485,15 @@
       <c r="D30">
         <v>43.064999999999998</v>
       </c>
-      <c r="F30">
+      <c r="E30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G30">
+      <c r="F30">
         <v>43.064999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -16498,15 +16503,15 @@
       <c r="D31">
         <v>47.218000000000004</v>
       </c>
-      <c r="F31">
+      <c r="E31">
         <f t="shared" si="0"/>
         <v>2.0457140589408676</v>
       </c>
-      <c r="G31">
+      <c r="F31">
         <v>47.218000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -16516,15 +16521,15 @@
       <c r="D32">
         <v>40.201000000000001</v>
       </c>
-      <c r="F32">
+      <c r="E32">
         <f t="shared" si="0"/>
         <v>0.3222192947339193</v>
       </c>
-      <c r="G32">
+      <c r="F32">
         <v>40.201000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -16534,15 +16539,15 @@
       <c r="D33">
         <v>45.811999999999998</v>
       </c>
-      <c r="F33">
+      <c r="E33">
         <f t="shared" si="0"/>
         <v>1.1172712956557642</v>
       </c>
-      <c r="G33">
+      <c r="F33">
         <v>45.811999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -16552,15 +16557,15 @@
       <c r="D34">
         <v>41.372</v>
       </c>
-      <c r="F34">
+      <c r="E34">
         <f t="shared" si="0"/>
         <v>1.7331972651065695</v>
       </c>
-      <c r="G34">
+      <c r="F34">
         <v>41.372</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -16570,15 +16575,15 @@
       <c r="D35">
         <v>40.880000000000003</v>
       </c>
-      <c r="F35">
+      <c r="E35">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G35">
+      <c r="F35">
         <v>40.880000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -16588,15 +16593,15 @@
       <c r="D36">
         <v>34.095999999999997</v>
       </c>
-      <c r="F36">
+      <c r="E36">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G36">
+      <c r="F36">
         <v>34.095999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -16606,15 +16611,15 @@
       <c r="D37">
         <v>34.835999999999999</v>
       </c>
-      <c r="F37">
+      <c r="E37">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G37">
+      <c r="F37">
         <v>34.835999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -16624,15 +16629,15 @@
       <c r="D38">
         <v>38.988999999999997</v>
       </c>
-      <c r="F38">
+      <c r="E38">
         <f t="shared" si="0"/>
         <v>1.1172712956557642</v>
       </c>
-      <c r="G38">
+      <c r="F38">
         <v>38.988999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -16642,15 +16647,15 @@
       <c r="D39">
         <v>38.140999999999998</v>
       </c>
-      <c r="F39">
+      <c r="E39">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G39">
+      <c r="F39">
         <v>38.140999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -16660,15 +16665,15 @@
       <c r="D40">
         <v>31.143999999999998</v>
       </c>
-      <c r="F40">
+      <c r="E40">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G40">
+      <c r="F40">
         <v>31.143999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -16678,15 +16683,15 @@
       <c r="D41">
         <v>36.359000000000002</v>
       </c>
-      <c r="F41">
+      <c r="E41">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G41">
+      <c r="F41">
         <v>36.359000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -16696,15 +16701,15 @@
       <c r="D42">
         <v>37.93</v>
       </c>
-      <c r="F42">
+      <c r="E42">
         <f t="shared" si="0"/>
         <v>2.8035253955765325</v>
       </c>
-      <c r="G42">
+      <c r="F42">
         <v>37.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -16714,15 +16719,15 @@
       <c r="D43">
         <v>39.872</v>
       </c>
-      <c r="F43">
+      <c r="E43">
         <f t="shared" si="0"/>
         <v>1.5453071164658241</v>
       </c>
-      <c r="G43">
+      <c r="F43">
         <v>39.872</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -16732,15 +16737,15 @@
       <c r="D44">
         <v>38.365000000000002</v>
       </c>
-      <c r="F44">
+      <c r="E44">
         <f t="shared" si="0"/>
         <v>1.2329961103921538</v>
       </c>
-      <c r="G44">
+      <c r="F44">
         <v>38.365000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -16750,15 +16755,15 @@
       <c r="D45">
         <v>40.624000000000002</v>
       </c>
-      <c r="F45">
+      <c r="E45">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G45">
+      <c r="F45">
         <v>40.624000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -16768,15 +16773,15 @@
       <c r="D46">
         <v>32.832000000000001</v>
       </c>
-      <c r="F46">
+      <c r="E46">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G46">
+      <c r="F46">
         <v>32.832000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -16786,15 +16791,15 @@
       <c r="D47">
         <v>30.175999999999998</v>
       </c>
-      <c r="F47">
+      <c r="E47">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G47">
+      <c r="F47">
         <v>30.175999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -16804,15 +16809,15 @@
       <c r="D48">
         <v>43.390999999999998</v>
       </c>
-      <c r="F48">
+      <c r="E48">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G48">
+      <c r="F48">
         <v>43.390999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -16822,15 +16827,15 @@
       <c r="D49">
         <v>32.932000000000002</v>
       </c>
-      <c r="F49">
+      <c r="E49">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G49">
+      <c r="F49">
         <v>32.932000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -16840,15 +16845,15 @@
       <c r="D50">
         <v>39.366</v>
       </c>
-      <c r="F50">
+      <c r="E50">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G50">
+      <c r="F50">
         <v>39.366</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -16858,15 +16863,15 @@
       <c r="D51">
         <v>39.994999999999997</v>
       </c>
-      <c r="F51">
+      <c r="E51">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G51">
+      <c r="F51">
         <v>39.994999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -16876,15 +16881,15 @@
       <c r="D52">
         <v>24.704000000000001</v>
       </c>
-      <c r="F52">
+      <c r="E52">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G52">
+      <c r="F52">
         <v>24.704000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -16894,15 +16899,15 @@
       <c r="D53">
         <v>35.277999999999999</v>
       </c>
-      <c r="F53">
+      <c r="E53">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G53">
+      <c r="F53">
         <v>35.277999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -16912,15 +16917,15 @@
       <c r="D54">
         <v>41.43</v>
       </c>
-      <c r="F54">
+      <c r="E54">
         <f t="shared" si="0"/>
         <v>2.0378247505883418</v>
       </c>
-      <c r="G54">
+      <c r="F54">
         <v>41.43</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -16930,15 +16935,15 @@
       <c r="D55">
         <v>40.159999999999997</v>
       </c>
-      <c r="F55">
+      <c r="E55">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G55">
+      <c r="F55">
         <v>40.159999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -16948,15 +16953,15 @@
       <c r="D56">
         <v>37.911999999999999</v>
       </c>
-      <c r="F56">
+      <c r="E56">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G56">
+      <c r="F56">
         <v>37.911999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -16966,15 +16971,15 @@
       <c r="D57">
         <v>41.578000000000003</v>
       </c>
-      <c r="F57">
+      <c r="E57">
         <f t="shared" si="0"/>
         <v>0.95904139232109353</v>
       </c>
-      <c r="G57">
+      <c r="F57">
         <v>41.578000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -16984,15 +16989,15 @@
       <c r="D58">
         <v>39.829000000000001</v>
       </c>
-      <c r="F58">
+      <c r="E58">
         <f t="shared" si="0"/>
         <v>1.909020854211156</v>
       </c>
-      <c r="G58">
+      <c r="F58">
         <v>39.829000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -17002,15 +17007,15 @@
       <c r="D59">
         <v>39.206000000000003</v>
       </c>
-      <c r="F59">
+      <c r="E59">
         <f t="shared" si="0"/>
         <v>2.9004217534577377</v>
       </c>
-      <c r="G59">
+      <c r="F59">
         <v>39.206000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -17020,15 +17025,15 @@
       <c r="D60">
         <v>40.344999999999999</v>
       </c>
-      <c r="F60">
+      <c r="E60">
         <f t="shared" si="0"/>
         <v>2.7050936105478733</v>
       </c>
-      <c r="G60">
+      <c r="F60">
         <v>40.344999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -17038,15 +17043,15 @@
       <c r="D61">
         <v>35.170999999999999</v>
       </c>
-      <c r="F61">
+      <c r="E61">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G61">
+      <c r="F61">
         <v>35.170999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -17056,15 +17061,15 @@
       <c r="D62">
         <v>39.383000000000003</v>
       </c>
-      <c r="F62">
+      <c r="E62">
         <f t="shared" si="0"/>
         <v>0.85125834871907524</v>
       </c>
-      <c r="G62">
+      <c r="F62">
         <v>39.383000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -17074,15 +17079,15 @@
       <c r="D63">
         <v>40.200000000000003</v>
       </c>
-      <c r="F63">
+      <c r="E63">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G63">
+      <c r="F63">
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -17092,15 +17097,15 @@
       <c r="D64">
         <v>38.412999999999997</v>
       </c>
-      <c r="F64">
+      <c r="E64">
         <f t="shared" si="0"/>
         <v>2.1849751906982608</v>
       </c>
-      <c r="G64">
+      <c r="F64">
         <v>38.412999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -17110,15 +17115,15 @@
       <c r="D65">
         <v>37.645000000000003</v>
       </c>
-      <c r="F65">
+      <c r="E65">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G65">
+      <c r="F65">
         <v>37.645000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>117</v>
       </c>
@@ -17128,15 +17133,15 @@
       <c r="D66">
         <v>39.076000000000001</v>
       </c>
-      <c r="F66">
+      <c r="E66">
         <f t="shared" si="0"/>
         <v>1.7566361082458481</v>
       </c>
-      <c r="G66">
+      <c r="F66">
         <v>39.076000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -17146,15 +17151,15 @@
       <c r="D67">
         <v>39.006</v>
       </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E68" si="1">LOG(C67 +0.1)</f>
+        <v>2.1525940779274699</v>
+      </c>
       <c r="F67">
-        <f t="shared" ref="F67:F68" si="1">LOG(C67 +0.1)</f>
-        <v>2.1525940779274699</v>
-      </c>
-      <c r="G67">
         <v>39.006</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -17164,11 +17169,11 @@
       <c r="D68">
         <v>36.075000000000003</v>
       </c>
-      <c r="F68">
+      <c r="E68">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G68">
+      <c r="F68">
         <v>36.075000000000003</v>
       </c>
     </row>
@@ -17179,20 +17184,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E71F05F-FF4D-406D-928C-3BD990AF8A26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.20703125" customWidth="1"/>
-    <col min="7" max="7" width="14.20703125" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" customWidth="1"/>
+    <col min="7" max="7" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17212,7 +17217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -17232,7 +17237,7 @@
         <v>50.79</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -17252,7 +17257,7 @@
         <v>61.71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -17272,7 +17277,7 @@
         <v>48.49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -17292,7 +17297,7 @@
         <v>52.15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -17312,7 +17317,7 @@
         <v>45.89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -17332,7 +17337,7 @@
         <v>57.414999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -17352,7 +17357,7 @@
         <v>49.527000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -17372,7 +17377,7 @@
         <v>52.286999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -17392,7 +17397,7 @@
         <v>57.18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -17412,7 +17417,7 @@
         <v>49.857999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -17432,7 +17437,7 @@
         <v>52.777000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -17452,7 +17457,7 @@
         <v>52.121000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -17472,7 +17477,7 @@
         <v>54.314999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -17492,7 +17497,7 @@
         <v>60.801000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -17512,7 +17517,7 @@
         <v>61.424999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -17532,7 +17537,7 @@
         <v>50.677</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -17552,7 +17557,7 @@
         <v>50.408999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -17572,7 +17577,7 @@
         <v>53.64</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -17592,7 +17597,7 @@
         <v>52.945999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -17612,7 +17617,7 @@
         <v>53.945</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -17632,7 +17637,7 @@
         <v>54.009</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -17652,7 +17657,7 @@
         <v>59.42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -17672,7 +17677,7 @@
         <v>63.73</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -17692,7 +17697,7 @@
         <v>51.954999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -17712,7 +17717,7 @@
         <v>59.773000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -17732,7 +17737,7 @@
         <v>52.698999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -17752,7 +17757,7 @@
         <v>52.033000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -17772,7 +17777,7 @@
         <v>49.853000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -17792,7 +17797,7 @@
         <v>47.268999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -17812,7 +17817,7 @@
         <v>52.353000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -17832,7 +17837,7 @@
         <v>50.692</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -17852,7 +17857,7 @@
         <v>53.398000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -17872,7 +17877,7 @@
         <v>46.265999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -17892,7 +17897,7 @@
         <v>50.677999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -17912,7 +17917,7 @@
         <v>62.79</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -17932,7 +17937,7 @@
         <v>54.701000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -17952,7 +17957,7 @@
         <v>52.445</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -17972,7 +17977,7 @@
         <v>52.774000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -17992,7 +17997,7 @@
         <v>60.204999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -18012,7 +18017,7 @@
         <v>57.715000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -18032,7 +18037,7 @@
         <v>51.743000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -18052,7 +18057,7 @@
         <v>51.341000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -18072,7 +18077,7 @@
         <v>55.271000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -18092,7 +18097,7 @@
         <v>49.323</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -18112,7 +18117,7 @@
         <v>61.735999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -18132,7 +18137,7 @@
         <v>63.43</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -18152,7 +18157,7 @@
         <v>53.969000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -18172,7 +18177,7 @@
         <v>58.512</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -18192,7 +18197,7 @@
         <v>51.636000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -18212,7 +18217,7 @@
         <v>50.27</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -18232,7 +18237,7 @@
         <v>72.02</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -18252,7 +18257,7 @@
         <v>55.712000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -18272,7 +18277,7 @@
         <v>49.685000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -18292,7 +18297,7 @@
         <v>53.36</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -18312,7 +18317,7 @@
         <v>51.46</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -18332,7 +18337,7 @@
         <v>48.735999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -18352,7 +18357,7 @@
         <v>52.734999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -18372,7 +18377,7 @@
         <v>51.796999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -18392,7 +18397,7 @@
         <v>51.533999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -18412,7 +18417,7 @@
         <v>54.857999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -18432,7 +18437,7 @@
         <v>51.898000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -18452,7 +18457,7 @@
         <v>54.003</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -18472,7 +18477,7 @@
         <v>52.633000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -18492,7 +18497,7 @@
         <v>52.662999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>117</v>
       </c>
@@ -18512,7 +18517,7 @@
         <v>51.109000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -18532,7 +18537,7 @@
         <v>53.718000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>

</xml_diff>